<commit_message>
show the ig template
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-us-core-tribal-affiliation.xlsx
+++ b/docs/StructureDefinition-us-core-tribal-affiliation.xlsx
@@ -268,63 +268,63 @@
 </t>
   </si>
   <si>
+    <t>Extension.id</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string
+</t>
+  </si>
+  <si>
+    <t>Unique id for inter-element referencing</t>
+  </si>
+  <si>
+    <t>Unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
+  </si>
+  <si>
+    <t>Element.id</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>Extension.extension</t>
+  </si>
+  <si>
+    <t>extensions
+user content</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension
+</t>
+  </si>
+  <si>
+    <t>Additional content defined by implementations</t>
+  </si>
+  <si>
+    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
+  </si>
+  <si>
+    <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value:url}
+</t>
+  </si>
+  <si>
+    <t>Extensions are always sliced by (at least) url</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>Element.extension</t>
+  </si>
+  <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
 ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
-  </si>
-  <si>
-    <t>Extension.id</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string
-</t>
-  </si>
-  <si>
-    <t>Unique id for inter-element referencing</t>
-  </si>
-  <si>
-    <t>Unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
-  </si>
-  <si>
-    <t>Element.id</t>
-  </si>
-  <si>
-    <t>n/a</t>
-  </si>
-  <si>
-    <t>Extension.extension</t>
-  </si>
-  <si>
-    <t>extensions
-user content</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extension
-</t>
-  </si>
-  <si>
-    <t>Additional content defined by implementations</t>
-  </si>
-  <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
-  </si>
-  <si>
-    <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value:url}
-</t>
-  </si>
-  <si>
-    <t>Extensions are always sliced by (at least) url</t>
-  </si>
-  <si>
-    <t>open</t>
-  </si>
-  <si>
-    <t>Element.extension</t>
   </si>
   <si>
     <t>tribalAffiliation</t>
@@ -1013,7 +1013,7 @@
         <v>82</v>
       </c>
       <c r="AI2" t="s" s="2">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="AJ2" t="s" s="2">
         <v>77</v>
@@ -1021,7 +1021,7 @@
     </row>
     <row r="3" hidden="true">
       <c r="A3" t="s" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s" s="2">
@@ -1032,25 +1032,25 @@
         <v>78</v>
       </c>
       <c r="F3" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="G3" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="H3" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="I3" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="J3" t="s" s="2">
         <v>85</v>
       </c>
-      <c r="G3" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="H3" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="I3" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="J3" t="s" s="2">
+      <c r="K3" t="s" s="2">
         <v>86</v>
       </c>
-      <c r="K3" t="s" s="2">
+      <c r="L3" t="s" s="2">
         <v>87</v>
-      </c>
-      <c r="L3" t="s" s="2">
-        <v>88</v>
       </c>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -1101,13 +1101,13 @@
         <v>77</v>
       </c>
       <c r="AE3" t="s" s="2">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AF3" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AG3" t="s" s="2">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AH3" t="s" s="2">
         <v>77</v>
@@ -1116,16 +1116,16 @@
         <v>77</v>
       </c>
       <c r="AJ3" t="s" s="2">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" hidden="true">
       <c r="A4" t="s" s="2">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s" s="2">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" t="s" s="2">
@@ -1144,16 +1144,16 @@
         <v>77</v>
       </c>
       <c r="J4" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="K4" t="s" s="2">
         <v>93</v>
       </c>
-      <c r="K4" t="s" s="2">
+      <c r="L4" t="s" s="2">
         <v>94</v>
       </c>
-      <c r="L4" t="s" s="2">
+      <c r="M4" t="s" s="2">
         <v>95</v>
-      </c>
-      <c r="M4" t="s" s="2">
-        <v>96</v>
       </c>
       <c r="N4" s="2"/>
       <c r="O4" t="s" s="2">
@@ -1191,19 +1191,19 @@
         <v>77</v>
       </c>
       <c r="AA4" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="AB4" t="s" s="2">
         <v>97</v>
       </c>
-      <c r="AB4" t="s" s="2">
+      <c r="AC4" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AD4" t="s" s="2">
         <v>98</v>
       </c>
-      <c r="AC4" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AD4" t="s" s="2">
+      <c r="AE4" t="s" s="2">
         <v>99</v>
-      </c>
-      <c r="AE4" t="s" s="2">
-        <v>100</v>
       </c>
       <c r="AF4" t="s" s="2">
         <v>78</v>
@@ -1215,15 +1215,15 @@
         <v>77</v>
       </c>
       <c r="AI4" t="s" s="2">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="AJ4" t="s" s="2">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B5" t="s" s="2">
         <v>101</v>
@@ -1233,10 +1233,10 @@
       </c>
       <c r="D5" s="2"/>
       <c r="E5" t="s" s="2">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F5" t="s" s="2">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G5" t="s" s="2">
         <v>102</v>
@@ -1248,7 +1248,7 @@
         <v>77</v>
       </c>
       <c r="J5" t="s" s="2">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K5" t="s" s="2">
         <v>103</v>
@@ -1305,7 +1305,7 @@
         <v>77</v>
       </c>
       <c r="AE5" t="s" s="2">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AF5" t="s" s="2">
         <v>78</v>
@@ -1317,7 +1317,7 @@
         <v>77</v>
       </c>
       <c r="AI5" t="s" s="2">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="AJ5" t="s" s="2">
         <v>77</v>
@@ -1336,25 +1336,25 @@
         <v>78</v>
       </c>
       <c r="F6" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="G6" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="H6" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="I6" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="J6" t="s" s="2">
         <v>85</v>
       </c>
-      <c r="G6" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="H6" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="I6" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="J6" t="s" s="2">
+      <c r="K6" t="s" s="2">
         <v>86</v>
       </c>
-      <c r="K6" t="s" s="2">
+      <c r="L6" t="s" s="2">
         <v>87</v>
-      </c>
-      <c r="L6" t="s" s="2">
-        <v>88</v>
       </c>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -1405,13 +1405,13 @@
         <v>77</v>
       </c>
       <c r="AE6" t="s" s="2">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AF6" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AG6" t="s" s="2">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AH6" t="s" s="2">
         <v>77</v>
@@ -1420,7 +1420,7 @@
         <v>77</v>
       </c>
       <c r="AJ6" t="s" s="2">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" hidden="true">
@@ -1429,7 +1429,7 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s" s="2">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" t="s" s="2">
@@ -1448,16 +1448,16 @@
         <v>77</v>
       </c>
       <c r="J7" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="K7" t="s" s="2">
         <v>93</v>
       </c>
-      <c r="K7" t="s" s="2">
+      <c r="L7" t="s" s="2">
         <v>94</v>
       </c>
-      <c r="L7" t="s" s="2">
+      <c r="M7" t="s" s="2">
         <v>95</v>
-      </c>
-      <c r="M7" t="s" s="2">
-        <v>96</v>
       </c>
       <c r="N7" s="2"/>
       <c r="O7" t="s" s="2">
@@ -1495,19 +1495,19 @@
         <v>77</v>
       </c>
       <c r="AA7" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="AB7" t="s" s="2">
         <v>97</v>
       </c>
-      <c r="AB7" t="s" s="2">
+      <c r="AC7" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AD7" t="s" s="2">
         <v>98</v>
       </c>
-      <c r="AC7" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AD7" t="s" s="2">
+      <c r="AE7" t="s" s="2">
         <v>99</v>
-      </c>
-      <c r="AE7" t="s" s="2">
-        <v>100</v>
       </c>
       <c r="AF7" t="s" s="2">
         <v>78</v>
@@ -1519,10 +1519,10 @@
         <v>77</v>
       </c>
       <c r="AI7" t="s" s="2">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="AJ7" t="s" s="2">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" hidden="true">
@@ -1535,10 +1535,10 @@
       </c>
       <c r="D8" s="2"/>
       <c r="E8" t="s" s="2">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F8" t="s" s="2">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G8" t="s" s="2">
         <v>77</v>
@@ -1612,10 +1612,10 @@
         <v>111</v>
       </c>
       <c r="AF8" t="s" s="2">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AG8" t="s" s="2">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AH8" t="s" s="2">
         <v>77</v>
@@ -1637,10 +1637,10 @@
       </c>
       <c r="D9" s="2"/>
       <c r="E9" t="s" s="2">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F9" t="s" s="2">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G9" t="s" s="2">
         <v>77</v>
@@ -1715,7 +1715,7 @@
         <v>78</v>
       </c>
       <c r="AG9" t="s" s="2">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AH9" t="s" s="2">
         <v>77</v>
@@ -1729,7 +1729,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B10" t="s" s="2">
         <v>122</v>
@@ -1742,7 +1742,7 @@
         <v>78</v>
       </c>
       <c r="F10" t="s" s="2">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G10" t="s" s="2">
         <v>102</v>
@@ -1754,7 +1754,7 @@
         <v>77</v>
       </c>
       <c r="J10" t="s" s="2">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K10" t="s" s="2">
         <v>123</v>
@@ -1811,7 +1811,7 @@
         <v>77</v>
       </c>
       <c r="AE10" t="s" s="2">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AF10" t="s" s="2">
         <v>78</v>
@@ -1823,7 +1823,7 @@
         <v>77</v>
       </c>
       <c r="AI10" t="s" s="2">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="AJ10" t="s" s="2">
         <v>77</v>
@@ -1842,25 +1842,25 @@
         <v>78</v>
       </c>
       <c r="F11" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="G11" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="H11" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="I11" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="J11" t="s" s="2">
         <v>85</v>
       </c>
-      <c r="G11" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="H11" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="I11" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="J11" t="s" s="2">
+      <c r="K11" t="s" s="2">
         <v>86</v>
       </c>
-      <c r="K11" t="s" s="2">
+      <c r="L11" t="s" s="2">
         <v>87</v>
-      </c>
-      <c r="L11" t="s" s="2">
-        <v>88</v>
       </c>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
@@ -1911,13 +1911,13 @@
         <v>77</v>
       </c>
       <c r="AE11" t="s" s="2">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AF11" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AG11" t="s" s="2">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AH11" t="s" s="2">
         <v>77</v>
@@ -1926,7 +1926,7 @@
         <v>77</v>
       </c>
       <c r="AJ11" t="s" s="2">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" hidden="true">
@@ -1935,7 +1935,7 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s" s="2">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" t="s" s="2">
@@ -1954,16 +1954,16 @@
         <v>77</v>
       </c>
       <c r="J12" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="K12" t="s" s="2">
         <v>93</v>
       </c>
-      <c r="K12" t="s" s="2">
+      <c r="L12" t="s" s="2">
         <v>94</v>
       </c>
-      <c r="L12" t="s" s="2">
+      <c r="M12" t="s" s="2">
         <v>95</v>
-      </c>
-      <c r="M12" t="s" s="2">
-        <v>96</v>
       </c>
       <c r="N12" s="2"/>
       <c r="O12" t="s" s="2">
@@ -2001,19 +2001,19 @@
         <v>77</v>
       </c>
       <c r="AA12" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="AB12" t="s" s="2">
         <v>97</v>
       </c>
-      <c r="AB12" t="s" s="2">
+      <c r="AC12" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AD12" t="s" s="2">
         <v>98</v>
       </c>
-      <c r="AC12" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AD12" t="s" s="2">
+      <c r="AE12" t="s" s="2">
         <v>99</v>
-      </c>
-      <c r="AE12" t="s" s="2">
-        <v>100</v>
       </c>
       <c r="AF12" t="s" s="2">
         <v>78</v>
@@ -2025,10 +2025,10 @@
         <v>77</v>
       </c>
       <c r="AI12" t="s" s="2">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="AJ12" t="s" s="2">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" hidden="true">
@@ -2041,10 +2041,10 @@
       </c>
       <c r="D13" s="2"/>
       <c r="E13" t="s" s="2">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F13" t="s" s="2">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G13" t="s" s="2">
         <v>77</v>
@@ -2118,10 +2118,10 @@
         <v>111</v>
       </c>
       <c r="AF13" t="s" s="2">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AG13" t="s" s="2">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AH13" t="s" s="2">
         <v>77</v>
@@ -2143,10 +2143,10 @@
       </c>
       <c r="D14" s="2"/>
       <c r="E14" t="s" s="2">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F14" t="s" s="2">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G14" t="s" s="2">
         <v>77</v>
@@ -2221,7 +2221,7 @@
         <v>78</v>
       </c>
       <c r="AG14" t="s" s="2">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AH14" t="s" s="2">
         <v>77</v>
@@ -2243,10 +2243,10 @@
       </c>
       <c r="D15" s="2"/>
       <c r="E15" t="s" s="2">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F15" t="s" s="2">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G15" t="s" s="2">
         <v>77</v>
@@ -2320,10 +2320,10 @@
         <v>111</v>
       </c>
       <c r="AF15" t="s" s="2">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AG15" t="s" s="2">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AH15" t="s" s="2">
         <v>77</v>
@@ -2423,7 +2423,7 @@
         <v>78</v>
       </c>
       <c r="AG16" t="s" s="2">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AH16" t="s" s="2">
         <v>77</v>

</xml_diff>